<commit_message>
:zap: add TC05 TC10
</commit_message>
<xml_diff>
--- a/FINAL_PROJECT/Work/Software_Testing_Plan.xlsx
+++ b/FINAL_PROJECT/Work/Software_Testing_Plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="111">
   <si>
     <t>Test Modules</t>
   </si>
@@ -26259,8 +26259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26736,7 +26736,9 @@
       <c r="F23" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="G23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>105</v>
+      </c>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
       <c r="J23" s="19"/>

</xml_diff>

<commit_message>
Test Plan mới nhất
</commit_message>
<xml_diff>
--- a/FINAL_PROJECT/Work/Software_Testing_Plan.xlsx
+++ b/FINAL_PROJECT/Work/Software_Testing_Plan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NhutNguyen\Desktop\software_testing\FINAL_PROJECT\Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iris Huynh\Documents\GitHub\Software-Testing\FINAL_PROJECT\Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD4AFE3-5F88-4CEC-A090-112F8DDA60CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phân công" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="112">
   <si>
     <t>Test Modules</t>
   </si>
@@ -410,11 +411,14 @@
   <si>
     <t>User can type special characters and symbols on the notepad editor window.</t>
   </si>
+  <si>
+    <t>Make sure there is a text file in "Public/Documents" with name ExampleTC11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1249,7 +1253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -26256,11 +26260,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26752,7 +26756,9 @@
       <c r="C24" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="18"/>
+      <c r="D24" s="18" t="s">
+        <v>111</v>
+      </c>
       <c r="E24" s="19" t="s">
         <v>83</v>
       </c>
@@ -26842,7 +26848,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G3 G5:G25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G3 G5:G25" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Passed, Failed, Blocked, Skipped"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>